<commit_message>
update: isDuplication (fix redundancy logic)
</commit_message>
<xml_diff>
--- a/nilai_raport_IPA - mini  duplication test.xlsx
+++ b/nilai_raport_IPA - mini  duplication test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="37">
   <si>
     <t>NO.</t>
   </si>
@@ -1128,10 +1128,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:CA13"/>
+  <dimension ref="A1:CA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="AJ4" workbookViewId="0">
-      <selection activeCell="BX14" sqref="BX14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A14" sqref="$A14:$XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.95" customHeight="1"/>
@@ -3136,7 +3136,7 @@
         <v>82</v>
       </c>
       <c r="D12" s="8">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="E12" s="8">
         <v>80</v>
@@ -3364,43 +3364,43 @@
     </row>
     <row r="13" ht="12.75" spans="1:79">
       <c r="A13" s="8">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C13" s="8">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="D13" s="8">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E13" s="8">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F13" s="8">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G13" s="8">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H13" s="8">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I13" s="8">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J13" s="8">
         <v>75</v>
       </c>
       <c r="K13" s="8">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L13" s="8">
         <v>73</v>
       </c>
       <c r="M13" s="8">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N13" s="8">
         <v>75</v>
@@ -3409,10 +3409,10 @@
         <v>75</v>
       </c>
       <c r="P13" s="8">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Q13" s="8">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R13" s="8">
         <v>83</v>
@@ -3427,16 +3427,16 @@
         <v>74</v>
       </c>
       <c r="V13" s="8">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="W13" s="8">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="X13" s="8">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Y13" s="8">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Z13" s="8">
         <v>77</v>
@@ -3454,10 +3454,10 @@
         <v>76</v>
       </c>
       <c r="AE13" s="8">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AF13" s="8">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AG13" s="8">
         <v>84</v>
@@ -3469,34 +3469,34 @@
         <v>85</v>
       </c>
       <c r="AJ13" s="8">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AK13" s="8">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AL13" s="8">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AM13" s="8">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AN13" s="8">
         <v>83</v>
       </c>
       <c r="AO13" s="8">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AP13" s="8">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AQ13" s="8">
         <v>80</v>
       </c>
       <c r="AR13" s="8">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AS13" s="8">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AT13" s="8">
         <v>79</v>
@@ -3505,43 +3505,43 @@
         <v>86</v>
       </c>
       <c r="AV13" s="8">
+        <v>85</v>
+      </c>
+      <c r="AW13" s="8">
+        <v>87</v>
+      </c>
+      <c r="AX13" s="8">
+        <v>78</v>
+      </c>
+      <c r="AY13" s="8">
+        <v>85</v>
+      </c>
+      <c r="AZ13" s="8">
+        <v>80</v>
+      </c>
+      <c r="BA13" s="8">
+        <v>83</v>
+      </c>
+      <c r="BB13" s="8">
         <v>86</v>
       </c>
-      <c r="AW13" s="8">
-        <v>88</v>
-      </c>
-      <c r="AX13" s="8">
-        <v>80</v>
-      </c>
-      <c r="AY13" s="8">
-        <v>86</v>
-      </c>
-      <c r="AZ13" s="8">
-        <v>82</v>
-      </c>
-      <c r="BA13" s="8">
-        <v>85</v>
-      </c>
-      <c r="BB13" s="8">
-        <v>85</v>
-      </c>
       <c r="BC13" s="8">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BD13" s="8">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="BE13" s="8">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="BF13" s="8">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="BG13" s="8">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="BH13" s="8">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BI13" s="8">
         <v>90</v>
@@ -3553,51 +3553,276 @@
         <v>88</v>
       </c>
       <c r="BL13" s="8">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="BM13" s="8">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="BN13" s="8">
         <v>90</v>
       </c>
       <c r="BO13" s="8">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="BP13" s="8">
         <v>87</v>
       </c>
       <c r="BQ13" s="8">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="BR13" s="8">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="BS13" s="8">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="BT13" s="8">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="BU13" s="8">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="BV13" s="8">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="BW13" s="16">
         <v>2023</v>
       </c>
-      <c r="BX13" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="BY13" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="BZ13" s="17" t="s">
-        <v>28</v>
-      </c>
+      <c r="BX13" s="17"/>
+      <c r="BY13" s="17"/>
+      <c r="BZ13" s="17"/>
       <c r="CA13" s="18"/>
+    </row>
+    <row r="14" ht="12.75" spans="1:79">
+      <c r="A14" s="8">
+        <v>32</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="8">
+        <v>100</v>
+      </c>
+      <c r="D14" s="8">
+        <v>80</v>
+      </c>
+      <c r="E14" s="8">
+        <v>81</v>
+      </c>
+      <c r="F14" s="8">
+        <v>73</v>
+      </c>
+      <c r="G14" s="8">
+        <v>79</v>
+      </c>
+      <c r="H14" s="8">
+        <v>73</v>
+      </c>
+      <c r="I14" s="8">
+        <v>76</v>
+      </c>
+      <c r="J14" s="8">
+        <v>75</v>
+      </c>
+      <c r="K14" s="8">
+        <v>77</v>
+      </c>
+      <c r="L14" s="8">
+        <v>73</v>
+      </c>
+      <c r="M14" s="8">
+        <v>77</v>
+      </c>
+      <c r="N14" s="8">
+        <v>75</v>
+      </c>
+      <c r="O14" s="8">
+        <v>75</v>
+      </c>
+      <c r="P14" s="8">
+        <v>74</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>73</v>
+      </c>
+      <c r="R14" s="8">
+        <v>83</v>
+      </c>
+      <c r="S14" s="8">
+        <v>81</v>
+      </c>
+      <c r="T14" s="8">
+        <v>82</v>
+      </c>
+      <c r="U14" s="8">
+        <v>74</v>
+      </c>
+      <c r="V14" s="8">
+        <v>82</v>
+      </c>
+      <c r="W14" s="8">
+        <v>75</v>
+      </c>
+      <c r="X14" s="8">
+        <v>77</v>
+      </c>
+      <c r="Y14" s="8">
+        <v>77</v>
+      </c>
+      <c r="Z14" s="8">
+        <v>77</v>
+      </c>
+      <c r="AA14" s="8">
+        <v>74</v>
+      </c>
+      <c r="AB14" s="8">
+        <v>77</v>
+      </c>
+      <c r="AC14" s="8">
+        <v>76</v>
+      </c>
+      <c r="AD14" s="8">
+        <v>76</v>
+      </c>
+      <c r="AE14" s="8">
+        <v>75</v>
+      </c>
+      <c r="AF14" s="8">
+        <v>76</v>
+      </c>
+      <c r="AG14" s="8">
+        <v>84</v>
+      </c>
+      <c r="AH14" s="8">
+        <v>83</v>
+      </c>
+      <c r="AI14" s="8">
+        <v>85</v>
+      </c>
+      <c r="AJ14" s="8">
+        <v>76</v>
+      </c>
+      <c r="AK14" s="8">
+        <v>84</v>
+      </c>
+      <c r="AL14" s="8">
+        <v>78</v>
+      </c>
+      <c r="AM14" s="8">
+        <v>80</v>
+      </c>
+      <c r="AN14" s="8">
+        <v>83</v>
+      </c>
+      <c r="AO14" s="8">
+        <v>81</v>
+      </c>
+      <c r="AP14" s="8">
+        <v>76</v>
+      </c>
+      <c r="AQ14" s="8">
+        <v>80</v>
+      </c>
+      <c r="AR14" s="8">
+        <v>76</v>
+      </c>
+      <c r="AS14" s="8">
+        <v>77</v>
+      </c>
+      <c r="AT14" s="8">
+        <v>79</v>
+      </c>
+      <c r="AU14" s="8">
+        <v>86</v>
+      </c>
+      <c r="AV14" s="8">
+        <v>85</v>
+      </c>
+      <c r="AW14" s="8">
+        <v>87</v>
+      </c>
+      <c r="AX14" s="8">
+        <v>78</v>
+      </c>
+      <c r="AY14" s="8">
+        <v>85</v>
+      </c>
+      <c r="AZ14" s="8">
+        <v>80</v>
+      </c>
+      <c r="BA14" s="8">
+        <v>83</v>
+      </c>
+      <c r="BB14" s="8">
+        <v>86</v>
+      </c>
+      <c r="BC14" s="8">
+        <v>81</v>
+      </c>
+      <c r="BD14" s="8">
+        <v>77</v>
+      </c>
+      <c r="BE14" s="8">
+        <v>79</v>
+      </c>
+      <c r="BF14" s="8">
+        <v>78</v>
+      </c>
+      <c r="BG14" s="8">
+        <v>78</v>
+      </c>
+      <c r="BH14" s="8">
+        <v>81</v>
+      </c>
+      <c r="BI14" s="8">
+        <v>90</v>
+      </c>
+      <c r="BJ14" s="8">
+        <v>85</v>
+      </c>
+      <c r="BK14" s="8">
+        <v>88</v>
+      </c>
+      <c r="BL14" s="8">
+        <v>81</v>
+      </c>
+      <c r="BM14" s="8">
+        <v>85</v>
+      </c>
+      <c r="BN14" s="8">
+        <v>90</v>
+      </c>
+      <c r="BO14" s="8">
+        <v>84</v>
+      </c>
+      <c r="BP14" s="8">
+        <v>87</v>
+      </c>
+      <c r="BQ14" s="8">
+        <v>85</v>
+      </c>
+      <c r="BR14" s="8">
+        <v>82</v>
+      </c>
+      <c r="BS14" s="8">
+        <v>83</v>
+      </c>
+      <c r="BT14" s="8">
+        <v>80</v>
+      </c>
+      <c r="BU14" s="8">
+        <v>80</v>
+      </c>
+      <c r="BV14" s="8">
+        <v>83</v>
+      </c>
+      <c r="BW14" s="16">
+        <v>2023</v>
+      </c>
+      <c r="BX14" s="17"/>
+      <c r="BY14" s="17"/>
+      <c r="BZ14" s="17"/>
+      <c r="CA14" s="18"/>
     </row>
   </sheetData>
   <sortState ref="A5:BX36">

</xml_diff>

<commit_message>
update: CollegeModel (redesign jurusan & universitas tables)
</commit_message>
<xml_diff>
--- a/nilai_raport_IPA - mini  duplication test.xlsx
+++ b/nilai_raport_IPA - mini  duplication test.xlsx
@@ -1131,18 +1131,18 @@
   <dimension ref="A1:CA14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="$A14:$XFD14"/>
+      <selection activeCell="BX9" sqref="BX9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="5.85714285714286" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.647619047619" style="1" customWidth="1"/>
     <col min="3" max="32" width="5.28571428571429" style="1" customWidth="1"/>
     <col min="33" max="46" width="4.71428571428571" style="1" customWidth="1"/>
     <col min="47" max="60" width="4.28571428571429" style="1" customWidth="1"/>
     <col min="61" max="74" width="4.57142857142857" style="1" customWidth="1"/>
-    <col min="75" max="75" width="9.14285714285714" style="1"/>
+    <col min="75" max="75" width="9.14285714285714" style="1" customWidth="1"/>
     <col min="76" max="76" width="43.2571428571429" style="2" customWidth="1"/>
     <col min="77" max="77" width="23.8666666666667" style="2" customWidth="1"/>
     <col min="78" max="78" width="28.7809523809524" style="2" customWidth="1"/>

</xml_diff>